<commit_message>
added more heteroskedasticity plots
</commit_message>
<xml_diff>
--- a/data/tests/unconditional_heteroskedasticity.xlsx
+++ b/data/tests/unconditional_heteroskedasticity.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0881881a0a4a5542/Documenten/GitHub/Crypto_Forecasting/data/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_0C09778E5B90DD33FBF92711595ED87656CD8A07" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{717E0855-01F3-46B8-946C-57D31D5177E8}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="11_0C09778E5B90DD33FBF92711595ED87656CD8A07" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28B53901-B1EF-45BC-98A7-E6CCE9BA6E0B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="47">
   <si>
     <t>Coin</t>
   </si>
@@ -146,6 +147,27 @@
   <si>
     <t>Count of Coin</t>
   </si>
+  <si>
+    <t>1-minute</t>
+  </si>
+  <si>
+    <t>15-minute</t>
+  </si>
+  <si>
+    <t>4-hour</t>
+  </si>
+  <si>
+    <t>1-day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADA15, ALGO15, ATOM15, BNB15, Eos15, ETC15,link15, ltc15, matic15,neo4h, </t>
+  </si>
+  <si>
+    <t>Count of Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALGO, ATOM, BNB, CHZ, LINK, LTC, MATIC, </t>
+  </si>
 </sst>
 </file>
 
@@ -209,10 +231,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -274,13 +296,11 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="75000"/>
@@ -330,13 +350,11 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="75000"/>
@@ -399,16 +417,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1m</c:v>
+                  <c:v>1-minute</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15m</c:v>
+                  <c:v>15-minute</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4h</c:v>
+                  <c:v>4-hour</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1d</c:v>
+                  <c:v>1-day</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -470,16 +488,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1m</c:v>
+                  <c:v>1-minute</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15m</c:v>
+                  <c:v>15-minute</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4h</c:v>
+                  <c:v>4-hour</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1d</c:v>
+                  <c:v>1-day</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -525,6 +543,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time frame</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -547,7 +620,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -590,6 +663,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of datasets</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -606,7 +734,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -648,7 +776,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -695,7 +823,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1100"/>
       </a:pPr>
       <a:endParaRPr lang="en-NL"/>
     </a:p>
@@ -712,7 +840,6 @@
         <c14:dropZoneCategories val="1"/>
         <c14:dropZoneData val="1"/>
         <c14:dropZoneSeries val="1"/>
-        <c14:dropZonesVisible val="1"/>
       </c14:pivotOptions>
     </c:ext>
     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
@@ -1277,10 +1404,10 @@
       <xdr:rowOff>118110</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>118110</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1306,6 +1433,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2382,7 +2513,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D44C24FD-3D43-4C18-A883-9B9D0393D405}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D44C24FD-3D43-4C18-A883-9B9D0393D405}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F98" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -2759,16 +2890,16 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1CE70F26-638C-484D-85CD-424CB9F5A4D0}" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1CE70F26-638C-484D-85CD-424CB9F5A4D0}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:E10" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="5">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
+        <item n="1-minute" x="0"/>
+        <item n="15-minute" x="1"/>
+        <item n="4-hour" x="2"/>
+        <item n="1-day" x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2861,6 +2992,267 @@
       </pivotArea>
     </chartFormat>
   </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B726B2C6-EE3B-4624-92CC-8D78CC24C44D}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C65" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="22">
+        <item x="4"/>
+        <item x="15"/>
+        <item x="12"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="17"/>
+        <item x="5"/>
+        <item x="16"/>
+        <item x="8"/>
+        <item x="1"/>
+        <item x="18"/>
+        <item x="7"/>
+        <item x="10"/>
+        <item x="6"/>
+        <item x="19"/>
+        <item x="11"/>
+        <item x="14"/>
+        <item x="9"/>
+        <item x="13"/>
+        <item x="3"/>
+        <item x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="61">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Time" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -3158,10 +3550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C2A3C0-4334-4459-9560-3A0217D059B2}">
-  <dimension ref="A3:F98"/>
+  <dimension ref="A3:G98"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3176,7 +3568,7 @@
     <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>39</v>
       </c>
@@ -3184,7 +3576,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -3201,7 +3593,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -3212,251 +3604,238 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6">
         <v>3</v>
       </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4">
-        <v>1</v>
-      </c>
-      <c r="F7" s="4">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="4">
-        <v>1</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="4">
-        <v>1</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10">
         <v>4</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10">
         <v>4</v>
       </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="4">
-        <v>1</v>
-      </c>
-      <c r="F10" s="4">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="4">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1</v>
-      </c>
-      <c r="E11" s="4">
-        <v>1</v>
-      </c>
-      <c r="F11" s="4">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
-        <v>1</v>
-      </c>
-      <c r="C12" s="4">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="4">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="4">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4">
-        <v>1</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15">
         <v>4</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15">
         <v>4</v>
       </c>
-      <c r="D15" s="4">
-        <v>1</v>
-      </c>
-      <c r="E15" s="4">
-        <v>1</v>
-      </c>
-      <c r="F15" s="4">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="4">
-        <v>1</v>
-      </c>
-      <c r="C16" s="4">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4">
-        <v>1</v>
-      </c>
-      <c r="E16" s="4">
-        <v>1</v>
-      </c>
-      <c r="F16" s="4">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="4">
-        <v>1</v>
-      </c>
-      <c r="C17" s="4">
-        <v>1</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="F17">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="4">
-        <v>1</v>
-      </c>
-      <c r="C18" s="4">
-        <v>1</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="F18">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="4">
-        <v>1</v>
-      </c>
-      <c r="C19" s="4">
-        <v>1</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="F19">
         <v>1</v>
       </c>
     </row>
@@ -3464,87 +3843,81 @@
       <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20">
         <v>4</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20">
         <v>4</v>
       </c>
-      <c r="D20" s="4">
-        <v>1</v>
-      </c>
-      <c r="E20" s="4">
-        <v>1</v>
-      </c>
-      <c r="F20" s="4">
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="4">
-        <v>1</v>
-      </c>
-      <c r="C21" s="4">
-        <v>1</v>
-      </c>
-      <c r="D21" s="4">
-        <v>1</v>
-      </c>
-      <c r="E21" s="4">
-        <v>1</v>
-      </c>
-      <c r="F21" s="4">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-      <c r="C22" s="4">
-        <v>1</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="F22">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="4">
-        <v>1</v>
-      </c>
-      <c r="C23" s="4">
-        <v>1</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="F23">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="4">
-        <v>1</v>
-      </c>
-      <c r="C24" s="4">
-        <v>1</v>
-      </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="F24">
         <v>1</v>
       </c>
     </row>
@@ -3552,83 +3925,75 @@
       <c r="A25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25">
         <v>2</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25">
         <v>2</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25">
         <v>2</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25">
         <v>2</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4">
-        <v>1</v>
-      </c>
-      <c r="E26" s="4">
-        <v>1</v>
-      </c>
-      <c r="F26" s="4">
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="4">
-        <v>1</v>
-      </c>
-      <c r="C27" s="4">
-        <v>1</v>
-      </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="F27">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="4">
-        <v>1</v>
-      </c>
-      <c r="C28" s="4">
-        <v>1</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="F28">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4">
-        <v>1</v>
-      </c>
-      <c r="E29" s="4">
-        <v>1</v>
-      </c>
-      <c r="F29" s="4">
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
         <v>1</v>
       </c>
     </row>
@@ -3636,79 +4001,69 @@
       <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30">
         <v>4</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30">
         <v>4</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4">
+      <c r="F30">
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="4">
-        <v>1</v>
-      </c>
-      <c r="C31" s="4">
-        <v>1</v>
-      </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="F31">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="4">
-        <v>1</v>
-      </c>
-      <c r="C32" s="4">
-        <v>1</v>
-      </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="F32">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="4">
-        <v>1</v>
-      </c>
-      <c r="C33" s="4">
-        <v>1</v>
-      </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="F33">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="4">
-        <v>1</v>
-      </c>
-      <c r="C34" s="4">
-        <v>1</v>
-      </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4">
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="F34">
         <v>1</v>
       </c>
     </row>
@@ -3716,47 +4071,41 @@
       <c r="A35" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35">
         <v>2</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35">
         <v>2</v>
       </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4">
+      <c r="F35">
         <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="4">
-        <v>1</v>
-      </c>
-      <c r="C36" s="4">
-        <v>1</v>
-      </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="F36">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="4">
-        <v>1</v>
-      </c>
-      <c r="C37" s="4">
-        <v>1</v>
-      </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4">
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="F37">
         <v>1</v>
       </c>
     </row>
@@ -3764,87 +4113,81 @@
       <c r="A38" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38">
         <v>3</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38">
         <v>3</v>
       </c>
-      <c r="D38" s="4">
+      <c r="D38">
         <v>2</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38">
         <v>2</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B39" s="4">
-        <v>1</v>
-      </c>
-      <c r="C39" s="4">
-        <v>1</v>
-      </c>
-      <c r="D39" s="4">
-        <v>1</v>
-      </c>
-      <c r="E39" s="4">
-        <v>1</v>
-      </c>
-      <c r="F39" s="4">
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
         <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="4">
-        <v>1</v>
-      </c>
-      <c r="C40" s="4">
-        <v>1</v>
-      </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4">
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="F40">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="4">
-        <v>1</v>
-      </c>
-      <c r="C41" s="4">
-        <v>1</v>
-      </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4">
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="F41">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4">
-        <v>1</v>
-      </c>
-      <c r="E42" s="4">
-        <v>1</v>
-      </c>
-      <c r="F42" s="4">
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
         <v>1</v>
       </c>
     </row>
@@ -3852,55 +4195,53 @@
       <c r="A43" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B43">
         <v>2</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43">
         <v>2</v>
       </c>
-      <c r="D43" s="4">
-        <v>1</v>
-      </c>
-      <c r="E43" s="4">
-        <v>1</v>
-      </c>
-      <c r="F43" s="4">
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
         <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="4">
-        <v>1</v>
-      </c>
-      <c r="C44" s="4">
-        <v>1</v>
-      </c>
-      <c r="D44" s="4">
-        <v>1</v>
-      </c>
-      <c r="E44" s="4">
-        <v>1</v>
-      </c>
-      <c r="F44" s="4">
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B45" s="4">
-        <v>1</v>
-      </c>
-      <c r="C45" s="4">
-        <v>1</v>
-      </c>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4">
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="F45">
         <v>1</v>
       </c>
     </row>
@@ -3908,83 +4249,75 @@
       <c r="A46" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46">
         <v>3</v>
       </c>
-      <c r="C46" s="4">
+      <c r="C46">
         <v>3</v>
       </c>
-      <c r="D46" s="4">
-        <v>1</v>
-      </c>
-      <c r="E46" s="4">
-        <v>1</v>
-      </c>
-      <c r="F46" s="4">
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
         <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4">
-        <v>1</v>
-      </c>
-      <c r="E47" s="4">
-        <v>1</v>
-      </c>
-      <c r="F47" s="4">
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B48" s="4">
-        <v>1</v>
-      </c>
-      <c r="C48" s="4">
-        <v>1</v>
-      </c>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4">
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="F48">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B49" s="4">
-        <v>1</v>
-      </c>
-      <c r="C49" s="4">
-        <v>1</v>
-      </c>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4">
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="F49">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B50" s="4">
-        <v>1</v>
-      </c>
-      <c r="C50" s="4">
-        <v>1</v>
-      </c>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4">
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="F50">
         <v>1</v>
       </c>
     </row>
@@ -3992,83 +4325,75 @@
       <c r="A51" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B51" s="4">
+      <c r="B51">
         <v>3</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C51">
         <v>3</v>
       </c>
-      <c r="D51" s="4">
-        <v>1</v>
-      </c>
-      <c r="E51" s="4">
-        <v>1</v>
-      </c>
-      <c r="F51" s="4">
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51">
         <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B52" s="4">
-        <v>1</v>
-      </c>
-      <c r="C52" s="4">
-        <v>1</v>
-      </c>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4">
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="F52">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="4">
-        <v>1</v>
-      </c>
-      <c r="C53" s="4">
-        <v>1</v>
-      </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4">
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="F53">
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="4">
-        <v>1</v>
-      </c>
-      <c r="C54" s="4">
-        <v>1</v>
-      </c>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4">
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="F54">
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4">
-        <v>1</v>
-      </c>
-      <c r="E55" s="4">
-        <v>1</v>
-      </c>
-      <c r="F55" s="4">
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
         <v>1</v>
       </c>
     </row>
@@ -4076,87 +4401,81 @@
       <c r="A56" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B56" s="4">
+      <c r="B56">
         <v>4</v>
       </c>
-      <c r="C56" s="4">
+      <c r="C56">
         <v>4</v>
       </c>
-      <c r="D56" s="4">
-        <v>1</v>
-      </c>
-      <c r="E56" s="4">
-        <v>1</v>
-      </c>
-      <c r="F56" s="4">
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56">
         <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B57" s="4">
-        <v>1</v>
-      </c>
-      <c r="C57" s="4">
-        <v>1</v>
-      </c>
-      <c r="D57" s="4">
-        <v>1</v>
-      </c>
-      <c r="E57" s="4">
-        <v>1</v>
-      </c>
-      <c r="F57" s="4">
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
         <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B58" s="4">
-        <v>1</v>
-      </c>
-      <c r="C58" s="4">
-        <v>1</v>
-      </c>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4">
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="F58">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B59" s="4">
-        <v>1</v>
-      </c>
-      <c r="C59" s="4">
-        <v>1</v>
-      </c>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4">
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="F59">
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B60" s="4">
-        <v>1</v>
-      </c>
-      <c r="C60" s="4">
-        <v>1</v>
-      </c>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4">
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="F60">
         <v>1</v>
       </c>
     </row>
@@ -4164,87 +4483,81 @@
       <c r="A61" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B61" s="4">
+      <c r="B61">
         <v>4</v>
       </c>
-      <c r="C61" s="4">
+      <c r="C61">
         <v>4</v>
       </c>
-      <c r="D61" s="4">
-        <v>1</v>
-      </c>
-      <c r="E61" s="4">
-        <v>1</v>
-      </c>
-      <c r="F61" s="4">
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
         <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="4">
-        <v>1</v>
-      </c>
-      <c r="C62" s="4">
-        <v>1</v>
-      </c>
-      <c r="D62" s="4">
-        <v>1</v>
-      </c>
-      <c r="E62" s="4">
-        <v>1</v>
-      </c>
-      <c r="F62" s="4">
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
         <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B63" s="4">
-        <v>1</v>
-      </c>
-      <c r="C63" s="4">
-        <v>1</v>
-      </c>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4">
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="F63">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
+      <c r="A64" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B64" s="4">
-        <v>1</v>
-      </c>
-      <c r="C64" s="4">
-        <v>1</v>
-      </c>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4">
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="F64">
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="5" t="s">
+      <c r="A65" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B65" s="4">
-        <v>1</v>
-      </c>
-      <c r="C65" s="4">
-        <v>1</v>
-      </c>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4">
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="F65">
         <v>1</v>
       </c>
     </row>
@@ -4252,87 +4565,81 @@
       <c r="A66" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B66" s="4">
+      <c r="B66">
         <v>4</v>
       </c>
-      <c r="C66" s="4">
+      <c r="C66">
         <v>4</v>
       </c>
-      <c r="D66" s="4">
-        <v>1</v>
-      </c>
-      <c r="E66" s="4">
-        <v>1</v>
-      </c>
-      <c r="F66" s="4">
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
         <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B67" s="4">
-        <v>1</v>
-      </c>
-      <c r="C67" s="4">
-        <v>1</v>
-      </c>
-      <c r="D67" s="4">
-        <v>1</v>
-      </c>
-      <c r="E67" s="4">
-        <v>1</v>
-      </c>
-      <c r="F67" s="4">
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67">
         <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="5" t="s">
+      <c r="A68" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B68" s="4">
-        <v>1</v>
-      </c>
-      <c r="C68" s="4">
-        <v>1</v>
-      </c>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
-      <c r="F68" s="4">
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="F68">
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="5" t="s">
+      <c r="A69" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B69" s="4">
-        <v>1</v>
-      </c>
-      <c r="C69" s="4">
-        <v>1</v>
-      </c>
-      <c r="D69" s="4"/>
-      <c r="E69" s="4"/>
-      <c r="F69" s="4">
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="F69">
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="5" t="s">
+      <c r="A70" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B70" s="4">
-        <v>1</v>
-      </c>
-      <c r="C70" s="4">
-        <v>1</v>
-      </c>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4">
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="F70">
         <v>1</v>
       </c>
     </row>
@@ -4340,71 +4647,67 @@
       <c r="A71" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B71" s="4">
+      <c r="B71">
         <v>3</v>
       </c>
-      <c r="C71" s="4">
+      <c r="C71">
         <v>3</v>
       </c>
-      <c r="D71" s="4">
-        <v>1</v>
-      </c>
-      <c r="E71" s="4">
-        <v>1</v>
-      </c>
-      <c r="F71" s="4">
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71">
         <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="5" t="s">
+      <c r="A72" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B72" s="4">
-        <v>1</v>
-      </c>
-      <c r="C72" s="4">
-        <v>1</v>
-      </c>
-      <c r="D72" s="4"/>
-      <c r="E72" s="4"/>
-      <c r="F72" s="4">
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="F72">
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B73" s="4">
-        <v>1</v>
-      </c>
-      <c r="C73" s="4">
-        <v>1</v>
-      </c>
-      <c r="D73" s="4"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="4">
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="F73">
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="5" t="s">
+      <c r="A74" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B74" s="4">
-        <v>1</v>
-      </c>
-      <c r="C74" s="4">
-        <v>1</v>
-      </c>
-      <c r="D74" s="4">
-        <v>1</v>
-      </c>
-      <c r="E74" s="4">
-        <v>1</v>
-      </c>
-      <c r="F74" s="4">
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74">
         <v>2</v>
       </c>
     </row>
@@ -4412,67 +4715,61 @@
       <c r="A75" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B75" s="4">
+      <c r="B75">
         <v>2</v>
       </c>
-      <c r="C75" s="4">
+      <c r="C75">
         <v>2</v>
       </c>
-      <c r="D75" s="4">
-        <v>1</v>
-      </c>
-      <c r="E75" s="4">
-        <v>1</v>
-      </c>
-      <c r="F75" s="4">
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="F75">
         <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="5" t="s">
+      <c r="A76" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B76" s="4"/>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4">
-        <v>1</v>
-      </c>
-      <c r="E76" s="4">
-        <v>1</v>
-      </c>
-      <c r="F76" s="4">
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76">
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="5" t="s">
+      <c r="A77" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B77" s="4">
-        <v>1</v>
-      </c>
-      <c r="C77" s="4">
-        <v>1</v>
-      </c>
-      <c r="D77" s="4"/>
-      <c r="E77" s="4"/>
-      <c r="F77" s="4">
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="F77">
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="5" t="s">
+      <c r="A78" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B78" s="4">
-        <v>1</v>
-      </c>
-      <c r="C78" s="4">
-        <v>1</v>
-      </c>
-      <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4">
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="F78">
         <v>1</v>
       </c>
     </row>
@@ -4480,67 +4777,61 @@
       <c r="A79" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B79" s="4">
+      <c r="B79">
         <v>2</v>
       </c>
-      <c r="C79" s="4">
+      <c r="C79">
         <v>2</v>
       </c>
-      <c r="D79" s="4">
-        <v>1</v>
-      </c>
-      <c r="E79" s="4">
-        <v>1</v>
-      </c>
-      <c r="F79" s="4">
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="F79">
         <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="5" t="s">
+      <c r="A80" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B80" s="4">
-        <v>1</v>
-      </c>
-      <c r="C80" s="4">
-        <v>1</v>
-      </c>
-      <c r="D80" s="4"/>
-      <c r="E80" s="4"/>
-      <c r="F80" s="4">
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="F80">
         <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="5" t="s">
+      <c r="A81" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B81" s="4">
-        <v>1</v>
-      </c>
-      <c r="C81" s="4">
-        <v>1</v>
-      </c>
-      <c r="D81" s="4"/>
-      <c r="E81" s="4"/>
-      <c r="F81" s="4">
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="F81">
         <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="5" t="s">
+      <c r="A82" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B82" s="4"/>
-      <c r="C82" s="4"/>
-      <c r="D82" s="4">
-        <v>1</v>
-      </c>
-      <c r="E82" s="4">
-        <v>1</v>
-      </c>
-      <c r="F82" s="4">
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="F82">
         <v>1</v>
       </c>
     </row>
@@ -4548,47 +4839,41 @@
       <c r="A83" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B83" s="4">
+      <c r="B83">
         <v>2</v>
       </c>
-      <c r="C83" s="4">
+      <c r="C83">
         <v>2</v>
       </c>
-      <c r="D83" s="4"/>
-      <c r="E83" s="4"/>
-      <c r="F83" s="4">
+      <c r="F83">
         <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="5" t="s">
+      <c r="A84" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B84" s="4">
-        <v>1</v>
-      </c>
-      <c r="C84" s="4">
-        <v>1</v>
-      </c>
-      <c r="D84" s="4"/>
-      <c r="E84" s="4"/>
-      <c r="F84" s="4">
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+      <c r="F84">
         <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="5" t="s">
+      <c r="A85" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B85" s="4">
-        <v>1</v>
-      </c>
-      <c r="C85" s="4">
-        <v>1</v>
-      </c>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="4">
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="F85">
         <v>1</v>
       </c>
     </row>
@@ -4596,67 +4881,61 @@
       <c r="A86" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B86" s="4">
+      <c r="B86">
         <v>2</v>
       </c>
-      <c r="C86" s="4">
+      <c r="C86">
         <v>2</v>
       </c>
-      <c r="D86" s="4">
-        <v>1</v>
-      </c>
-      <c r="E86" s="4">
-        <v>1</v>
-      </c>
-      <c r="F86" s="4">
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86">
         <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="5" t="s">
+      <c r="A87" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4">
-        <v>1</v>
-      </c>
-      <c r="E87" s="4">
-        <v>1</v>
-      </c>
-      <c r="F87" s="4">
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="F87">
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="5" t="s">
+      <c r="A88" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B88" s="4">
-        <v>1</v>
-      </c>
-      <c r="C88" s="4">
-        <v>1</v>
-      </c>
-      <c r="D88" s="4"/>
-      <c r="E88" s="4"/>
-      <c r="F88" s="4">
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+      <c r="F88">
         <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="5" t="s">
+      <c r="A89" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B89" s="4">
-        <v>1</v>
-      </c>
-      <c r="C89" s="4">
-        <v>1</v>
-      </c>
-      <c r="D89" s="4"/>
-      <c r="E89" s="4"/>
-      <c r="F89" s="4">
+      <c r="B89">
+        <v>1</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="F89">
         <v>1</v>
       </c>
     </row>
@@ -4664,67 +4943,61 @@
       <c r="A90" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B90" s="4">
+      <c r="B90">
         <v>2</v>
       </c>
-      <c r="C90" s="4">
+      <c r="C90">
         <v>2</v>
       </c>
-      <c r="D90" s="4">
-        <v>1</v>
-      </c>
-      <c r="E90" s="4">
-        <v>1</v>
-      </c>
-      <c r="F90" s="4">
+      <c r="D90">
+        <v>1</v>
+      </c>
+      <c r="E90">
+        <v>1</v>
+      </c>
+      <c r="F90">
         <v>3</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91" s="5" t="s">
+      <c r="A91" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B91" s="4"/>
-      <c r="C91" s="4"/>
-      <c r="D91" s="4">
-        <v>1</v>
-      </c>
-      <c r="E91" s="4">
-        <v>1</v>
-      </c>
-      <c r="F91" s="4">
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="F91">
         <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92" s="5" t="s">
+      <c r="A92" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B92" s="4">
-        <v>1</v>
-      </c>
-      <c r="C92" s="4">
-        <v>1</v>
-      </c>
-      <c r="D92" s="4"/>
-      <c r="E92" s="4"/>
-      <c r="F92" s="4">
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="F92">
         <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93" s="5" t="s">
+      <c r="A93" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B93" s="4">
-        <v>1</v>
-      </c>
-      <c r="C93" s="4">
-        <v>1</v>
-      </c>
-      <c r="D93" s="4"/>
-      <c r="E93" s="4"/>
-      <c r="F93" s="4">
+      <c r="B93">
+        <v>1</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="F93">
         <v>1</v>
       </c>
     </row>
@@ -4732,67 +5005,61 @@
       <c r="A94" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B94" s="4">
+      <c r="B94">
         <v>2</v>
       </c>
-      <c r="C94" s="4">
+      <c r="C94">
         <v>2</v>
       </c>
-      <c r="D94" s="4">
-        <v>1</v>
-      </c>
-      <c r="E94" s="4">
-        <v>1</v>
-      </c>
-      <c r="F94" s="4">
+      <c r="D94">
+        <v>1</v>
+      </c>
+      <c r="E94">
+        <v>1</v>
+      </c>
+      <c r="F94">
         <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" s="5" t="s">
+      <c r="A95" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B95" s="4">
-        <v>1</v>
-      </c>
-      <c r="C95" s="4">
-        <v>1</v>
-      </c>
-      <c r="D95" s="4"/>
-      <c r="E95" s="4"/>
-      <c r="F95" s="4">
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="F95">
         <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="5" t="s">
+      <c r="A96" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B96" s="4">
-        <v>1</v>
-      </c>
-      <c r="C96" s="4">
-        <v>1</v>
-      </c>
-      <c r="D96" s="4"/>
-      <c r="E96" s="4"/>
-      <c r="F96" s="4">
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="F96">
         <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" s="5" t="s">
+      <c r="A97" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B97" s="4"/>
-      <c r="C97" s="4"/>
-      <c r="D97" s="4">
-        <v>1</v>
-      </c>
-      <c r="E97" s="4">
-        <v>1</v>
-      </c>
-      <c r="F97" s="4">
+      <c r="D97">
+        <v>1</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
+      <c r="F97">
         <v>1</v>
       </c>
     </row>
@@ -4800,19 +5067,19 @@
       <c r="A98" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B98" s="4">
+      <c r="B98">
         <v>61</v>
       </c>
-      <c r="C98" s="4">
+      <c r="C98">
         <v>61</v>
       </c>
-      <c r="D98" s="4">
+      <c r="D98">
         <v>20</v>
       </c>
-      <c r="E98" s="4">
+      <c r="E98">
         <v>20</v>
       </c>
-      <c r="F98" s="4">
+      <c r="F98">
         <v>81</v>
       </c>
     </row>
@@ -4825,8 +5092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF4986E-53F4-40E1-885A-D5F309A1ABB0}">
   <dimension ref="A3:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4873,65 +5140,63 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4">
+        <v>40</v>
+      </c>
+      <c r="B6">
         <v>21</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4">
+      <c r="D6">
         <v>21</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="4">
+        <v>41</v>
+      </c>
+      <c r="B7">
         <v>12</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7">
         <v>14</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7">
         <v>26</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="4">
-        <v>9</v>
-      </c>
-      <c r="C8" s="4">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4">
+        <v>42</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
         <v>15</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4">
+        <v>43</v>
+      </c>
+      <c r="B9">
         <v>19</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4">
+      <c r="D9">
         <v>19</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9">
         <v>19</v>
       </c>
     </row>
@@ -4939,16 +5204,16 @@
       <c r="A10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10">
         <v>61</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10">
         <v>20</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10">
         <v>81</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10">
         <v>81</v>
       </c>
     </row>
@@ -4959,6 +5224,719 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{084874DE-3F16-4AF6-A34C-D5150C59B0F6}">
+  <dimension ref="A3:E65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="5">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5">
+        <v>4</v>
+      </c>
+      <c r="C9" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="5">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="5">
+        <v>4</v>
+      </c>
+      <c r="C12" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5">
+        <v>5</v>
+      </c>
+      <c r="C14" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="5">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="5">
+        <v>4</v>
+      </c>
+      <c r="C17" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="5">
+        <v>2</v>
+      </c>
+      <c r="C18" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="5">
+        <v>2</v>
+      </c>
+      <c r="C19" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="5">
+        <v>4</v>
+      </c>
+      <c r="C20" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="5">
+        <v>4</v>
+      </c>
+      <c r="C21" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="5">
+        <v>2</v>
+      </c>
+      <c r="C22" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="5">
+        <v>2</v>
+      </c>
+      <c r="C23" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="5">
+        <v>5</v>
+      </c>
+      <c r="C24" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="5">
+        <v>3</v>
+      </c>
+      <c r="C25" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="5">
+        <v>2</v>
+      </c>
+      <c r="C26" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="5">
+        <v>3</v>
+      </c>
+      <c r="C27" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="5">
+        <v>2</v>
+      </c>
+      <c r="C28" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
+      <c r="C29" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="5">
+        <v>4</v>
+      </c>
+      <c r="C30" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="5">
+        <v>3</v>
+      </c>
+      <c r="C31" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="5">
+        <v>1</v>
+      </c>
+      <c r="C32" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="5">
+        <v>4</v>
+      </c>
+      <c r="C33" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="5">
+        <v>3</v>
+      </c>
+      <c r="C34" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="5">
+        <v>1</v>
+      </c>
+      <c r="C35" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="5">
+        <v>5</v>
+      </c>
+      <c r="C36" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="5">
+        <v>4</v>
+      </c>
+      <c r="C37" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="5">
+        <v>1</v>
+      </c>
+      <c r="C38" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="5">
+        <v>5</v>
+      </c>
+      <c r="C39" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="5">
+        <v>4</v>
+      </c>
+      <c r="C40" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" s="5">
+        <v>1</v>
+      </c>
+      <c r="C41" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="5">
+        <v>5</v>
+      </c>
+      <c r="C42" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="5">
+        <v>4</v>
+      </c>
+      <c r="C43" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="5">
+        <v>1</v>
+      </c>
+      <c r="C44" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" s="5">
+        <v>4</v>
+      </c>
+      <c r="C45" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="5">
+        <v>3</v>
+      </c>
+      <c r="C46" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="5">
+        <v>1</v>
+      </c>
+      <c r="C47" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="5">
+        <v>3</v>
+      </c>
+      <c r="C48" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="5">
+        <v>2</v>
+      </c>
+      <c r="C49" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50" s="5">
+        <v>1</v>
+      </c>
+      <c r="C50" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" s="5">
+        <v>3</v>
+      </c>
+      <c r="C51" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="5">
+        <v>2</v>
+      </c>
+      <c r="C52" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" s="5">
+        <v>1</v>
+      </c>
+      <c r="C53" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B54" s="5">
+        <v>2</v>
+      </c>
+      <c r="C54" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="5">
+        <v>2</v>
+      </c>
+      <c r="C55" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56" s="5">
+        <v>3</v>
+      </c>
+      <c r="C56" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="5">
+        <v>2</v>
+      </c>
+      <c r="C57" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B58" s="5">
+        <v>1</v>
+      </c>
+      <c r="C58" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B59" s="5">
+        <v>3</v>
+      </c>
+      <c r="C59" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="5">
+        <v>2</v>
+      </c>
+      <c r="C60" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61" s="5">
+        <v>1</v>
+      </c>
+      <c r="C61" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62" s="5">
+        <v>3</v>
+      </c>
+      <c r="C62" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="5">
+        <v>2</v>
+      </c>
+      <c r="C63" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B64" s="5">
+        <v>1</v>
+      </c>
+      <c r="C64" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B65" s="5">
+        <v>81</v>
+      </c>
+      <c r="C65" s="5">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D169"/>
   <sheetViews>

</xml_diff>